<commit_message>
[feat] Quest 1039까지 제작 완료
</commit_message>
<xml_diff>
--- a/excel2json-master/QuestScript_Data.xlsx
+++ b/excel2json-master/QuestScript_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B9F5EE-493E-491A-A478-F7DEBFC79501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CF26C5-F7CD-442E-BEB1-4F19FCDABED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A398EBC-9C4D-4430-B016-D61C1F5CC80E}"/>
   </bookViews>
@@ -1628,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38187CEB-C85B-4882-A8E4-E722601192A3}">
   <dimension ref="A1:E275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>

</xml_diff>